<commit_message>
Commit Login - Falta completar formulario
Commit Login - Falta completar formulario
</commit_message>
<xml_diff>
--- a/faltantes.xlsx
+++ b/faltantes.xlsx
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +449,7 @@
     <col min="2" max="2" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>

</xml_diff>